<commit_message>
Use a default parser if none exists
</commit_message>
<xml_diff>
--- a/spec/fixtures/contacts.xlsx
+++ b/spec/fixtures/contacts.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Number</t>
+    <t xml:space="preserve">Phone</t>
   </si>
   <si>
     <t xml:space="preserve">John Doe 1</t>
@@ -76,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,9 +166,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>